<commit_message>
update to damage_interp to include updated coordinates, DD-nearest neighbor, impervious cover
</commit_message>
<xml_diff>
--- a/S2_damage.xlsx
+++ b/S2_damage.xlsx
@@ -214,6 +214,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -301,13 +302,16 @@
   </sheetPr>
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C60"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -596,12 +600,12 @@
         <v>-79.93861111</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>4044194444</v>
+        <v>40.44194444</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>-79.93888889</v>

</xml_diff>